<commit_message>
Changed the localize handlebars function to expose the data model and the calculates
</commit_message>
<xml_diff>
--- a/app/tables/Ethiopia_members/forms/Ethiopia_Section2_other_info/Ethiopia_Section2_other_info.xlsx
+++ b/app/tables/Ethiopia_members/forms/Ethiopia_Section2_other_info/Ethiopia_Section2_other_info.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
@@ -367,30 +367,9 @@
     <t>string</t>
   </si>
   <si>
-    <t>What is {{name}}'s sex?</t>
-  </si>
-  <si>
     <t>Ethiopia_members</t>
   </si>
   <si>
-    <t>What is {{name}}'s relationship to the household head?</t>
-  </si>
-  <si>
-    <t>What is {{name}}'s age?</t>
-  </si>
-  <si>
-    <t>Marital status of {{name}}.</t>
-  </si>
-  <si>
-    <t>For how many months during the last 12 months was {{name}} away from the household?</t>
-  </si>
-  <si>
-    <t>In what region was {{name}} born?</t>
-  </si>
-  <si>
-    <t>What is {{name}}'s main religion?</t>
-  </si>
-  <si>
     <t>Ethiopia_Section2_other_info</t>
   </si>
   <si>
@@ -659,6 +638,27 @@
   </si>
   <si>
     <t>Section 2</t>
+  </si>
+  <si>
+    <t>What is {{data.name}}'s relationship to the household head?</t>
+  </si>
+  <si>
+    <t>What is {{data.name}}'s sex?</t>
+  </si>
+  <si>
+    <t>What is {{data.name}}'s age?</t>
+  </si>
+  <si>
+    <t>Marital status of {{data.name}}.</t>
+  </si>
+  <si>
+    <t>For how many months during the last 12 months was {{data.name}} away from the household?</t>
+  </si>
+  <si>
+    <t>In what region was {{data.name}} born?</t>
+  </si>
+  <si>
+    <t>What is {{data.name}}'s main religion?</t>
   </si>
 </sst>
 </file>
@@ -1293,23 +1293,23 @@
         <v>11</v>
       </c>
       <c r="D1" s="41" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="B3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C3" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D3" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -1327,8 +1327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1347,7 +1347,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="42" customFormat="1" ht="30">
       <c r="A1" s="42" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="B1" s="42" t="s">
         <v>21</v>
@@ -1371,18 +1371,18 @@
         <v>24</v>
       </c>
       <c r="I1" s="42" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="J1" s="42" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="K1" s="42" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="105">
       <c r="A2" s="1" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>14</v>
@@ -1394,7 +1394,7 @@
         <v>19</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>116</v>
+        <v>205</v>
       </c>
       <c r="I2" s="1" t="b">
         <v>1</v>
@@ -1411,7 +1411,7 @@
         <v>18</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>114</v>
+        <v>206</v>
       </c>
       <c r="I3" s="1" t="b">
         <v>1</v>
@@ -1419,7 +1419,7 @@
     </row>
     <row r="4" spans="1:11" ht="90">
       <c r="A4" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>9</v>
@@ -1428,7 +1428,7 @@
         <v>10</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>117</v>
+        <v>207</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>17</v>
@@ -1437,10 +1437,10 @@
         <v>1</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="53" customFormat="1" ht="16" customHeight="1">
@@ -1453,7 +1453,7 @@
     </row>
     <row r="6" spans="1:11" s="53" customFormat="1" ht="69" customHeight="1">
       <c r="A6" s="53" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="D6" s="53" t="s">
         <v>14</v>
@@ -1465,7 +1465,7 @@
         <v>12</v>
       </c>
       <c r="G6" s="53" t="s">
-        <v>118</v>
+        <v>208</v>
       </c>
       <c r="I6" s="54" t="s">
         <v>15</v>
@@ -1492,16 +1492,16 @@
         <v>73</v>
       </c>
       <c r="G9" s="48" t="s">
-        <v>119</v>
+        <v>209</v>
       </c>
       <c r="H9" s="48" t="s">
         <v>74</v>
       </c>
       <c r="J9" s="48" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="K9" s="48" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="48" customFormat="1">
@@ -1520,7 +1520,7 @@
         <v>76</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>120</v>
+        <v>210</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="45" customFormat="1">
@@ -1542,7 +1542,7 @@
         <v>111</v>
       </c>
       <c r="G13" s="45" t="s">
-        <v>121</v>
+        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="45" customFormat="1">
@@ -1565,7 +1565,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -2018,7 +2018,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -2043,7 +2043,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2051,7 +2051,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2059,7 +2059,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2084,7 +2084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A38" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -2097,7 +2097,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="52" customFormat="1">
       <c r="A1" s="50" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B1" s="51" t="s">
         <v>8</v>
@@ -2108,7 +2108,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>112</v>
@@ -2119,7 +2119,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="4" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>8</v>
@@ -2130,7 +2130,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="6" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>19</v>
@@ -2195,10 +2195,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="8" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>14</v>
@@ -2207,7 +2207,7 @@
     <row r="12" spans="1:3">
       <c r="A12" s="8"/>
       <c r="B12" s="9" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>14</v>
@@ -2216,16 +2216,16 @@
     <row r="13" spans="1:3">
       <c r="A13" s="8"/>
       <c r="B13" s="9" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="8"/>
       <c r="B14" s="9" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>14</v>
@@ -2234,7 +2234,7 @@
     <row r="15" spans="1:3">
       <c r="A15" s="8"/>
       <c r="B15" s="9" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>14</v>
@@ -2243,7 +2243,7 @@
     <row r="16" spans="1:3">
       <c r="A16" s="8"/>
       <c r="B16" s="9" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>113</v>
@@ -2252,7 +2252,7 @@
     <row r="17" spans="1:3">
       <c r="A17" s="8"/>
       <c r="B17" s="9" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>14</v>
@@ -2260,10 +2260,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="10" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>14</v>
@@ -2271,10 +2271,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="13" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C19" s="15" t="s">
         <v>14</v>
@@ -2283,7 +2283,7 @@
     <row r="20" spans="1:3">
       <c r="A20" s="13"/>
       <c r="B20" s="14" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>9</v>
@@ -2292,7 +2292,7 @@
     <row r="21" spans="1:3">
       <c r="A21" s="13"/>
       <c r="B21" s="14" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="C21" s="15" t="s">
         <v>9</v>
@@ -2301,7 +2301,7 @@
     <row r="22" spans="1:3">
       <c r="A22" s="13"/>
       <c r="B22" s="14" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C22" s="15" t="s">
         <v>9</v>
@@ -2310,7 +2310,7 @@
     <row r="23" spans="1:3">
       <c r="A23" s="13"/>
       <c r="B23" s="14" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>14</v>
@@ -2318,10 +2318,10 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="16" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C24" s="18" t="s">
         <v>9</v>
@@ -2330,7 +2330,7 @@
     <row r="25" spans="1:3">
       <c r="A25" s="16"/>
       <c r="B25" s="17" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C25" s="18" t="s">
         <v>9</v>
@@ -2339,7 +2339,7 @@
     <row r="26" spans="1:3">
       <c r="A26" s="16"/>
       <c r="B26" s="17" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C26" s="18" t="s">
         <v>9</v>
@@ -2347,10 +2347,10 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="19" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C27" s="21" t="s">
         <v>9</v>
@@ -2358,10 +2358,10 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="22" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C28" s="24" t="s">
         <v>9</v>
@@ -2369,10 +2369,10 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="25" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C29" s="27" t="s">
         <v>9</v>
@@ -2380,10 +2380,10 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="28" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="C30" s="30" t="s">
         <v>9</v>
@@ -2391,21 +2391,21 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="31" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="B31" s="32" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C31" s="32" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="33" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="B32" s="34" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C32" s="34" t="s">
         <v>87</v>
@@ -2414,7 +2414,7 @@
     <row r="33" spans="1:3">
       <c r="A33" s="33"/>
       <c r="B33" s="34" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="C33" s="34" t="s">
         <v>9</v>
@@ -2423,7 +2423,7 @@
     <row r="34" spans="1:3">
       <c r="A34" s="33"/>
       <c r="B34" s="34" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C34" s="34" t="s">
         <v>14</v>
@@ -2432,7 +2432,7 @@
     <row r="35" spans="1:3">
       <c r="A35" s="33"/>
       <c r="B35" s="34" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C35" s="34" t="s">
         <v>87</v>
@@ -2440,10 +2440,10 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="35" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="B36" s="36" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C36" s="36" t="s">
         <v>113</v>
@@ -2451,10 +2451,10 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="37" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="B37" s="38" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C37" s="38" t="s">
         <v>87</v>
@@ -2463,7 +2463,7 @@
     <row r="38" spans="1:3">
       <c r="A38" s="37"/>
       <c r="B38" s="38" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C38" s="38" t="s">
         <v>14</v>
@@ -2472,7 +2472,7 @@
     <row r="39" spans="1:3">
       <c r="A39" s="37"/>
       <c r="B39" s="38" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C39" s="38" t="s">
         <v>9</v>
@@ -2481,7 +2481,7 @@
     <row r="40" spans="1:3">
       <c r="A40" s="37"/>
       <c r="B40" s="38" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="C40" s="38" t="s">
         <v>14</v>
@@ -2490,7 +2490,7 @@
     <row r="41" spans="1:3">
       <c r="A41" s="37"/>
       <c r="B41" s="38" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C41" s="38" t="s">
         <v>14</v>
@@ -2499,7 +2499,7 @@
     <row r="42" spans="1:3">
       <c r="A42" s="37"/>
       <c r="B42" s="38" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C42" s="38" t="s">
         <v>9</v>
@@ -2508,7 +2508,7 @@
     <row r="43" spans="1:3">
       <c r="A43" s="37"/>
       <c r="B43" s="38" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C43" s="38" t="s">
         <v>14</v>
@@ -2516,10 +2516,10 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="13" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C44" s="15" t="s">
         <v>87</v>
@@ -2528,7 +2528,7 @@
     <row r="45" spans="1:3">
       <c r="A45" s="13"/>
       <c r="B45" s="15" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="C45" s="15" t="s">
         <v>14</v>
@@ -2537,7 +2537,7 @@
     <row r="46" spans="1:3">
       <c r="A46" s="13"/>
       <c r="B46" s="15" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="C46" s="15" t="s">
         <v>9</v>
@@ -2546,7 +2546,7 @@
     <row r="47" spans="1:3">
       <c r="A47" s="13"/>
       <c r="B47" s="15" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C47" s="15" t="s">
         <v>14</v>
@@ -2555,7 +2555,7 @@
     <row r="48" spans="1:3">
       <c r="A48" s="13"/>
       <c r="B48" s="15" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="C48" s="15" t="s">
         <v>14</v>
@@ -2564,7 +2564,7 @@
     <row r="49" spans="1:3">
       <c r="A49" s="13"/>
       <c r="B49" s="15" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="C49" s="15" t="s">
         <v>14</v>
@@ -2573,7 +2573,7 @@
     <row r="50" spans="1:3">
       <c r="A50" s="13"/>
       <c r="B50" s="15" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C50" s="15" t="s">
         <v>14</v>
@@ -2582,7 +2582,7 @@
     <row r="51" spans="1:3">
       <c r="A51" s="13"/>
       <c r="B51" s="15" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C51" s="15" t="s">
         <v>14</v>
@@ -2591,7 +2591,7 @@
     <row r="52" spans="1:3">
       <c r="A52" s="13"/>
       <c r="B52" s="15" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C52" s="15" t="s">
         <v>14</v>
@@ -2600,7 +2600,7 @@
     <row r="53" spans="1:3">
       <c r="A53" s="13"/>
       <c r="B53" s="15" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C53" s="15" t="s">
         <v>9</v>
@@ -2609,7 +2609,7 @@
     <row r="54" spans="1:3">
       <c r="A54" s="13"/>
       <c r="B54" s="15" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C54" s="15" t="s">
         <v>14</v>
@@ -2617,10 +2617,10 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="39" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="B55" s="40" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C55" s="40" t="s">
         <v>87</v>
@@ -2629,7 +2629,7 @@
     <row r="56" spans="1:3">
       <c r="A56" s="39"/>
       <c r="B56" s="40" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="C56" s="40" t="s">
         <v>14</v>
@@ -2638,7 +2638,7 @@
     <row r="57" spans="1:3">
       <c r="A57" s="39"/>
       <c r="B57" s="40" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C57" s="40" t="s">
         <v>9</v>
@@ -2647,7 +2647,7 @@
     <row r="58" spans="1:3">
       <c r="A58" s="39"/>
       <c r="B58" s="40" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C58" s="40" t="s">
         <v>14</v>
@@ -2656,7 +2656,7 @@
     <row r="59" spans="1:3">
       <c r="A59" s="39"/>
       <c r="B59" s="40" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="C59" s="40" t="s">
         <v>14</v>
@@ -2665,7 +2665,7 @@
     <row r="60" spans="1:3">
       <c r="A60" s="39"/>
       <c r="B60" s="40" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C60" s="40" t="s">
         <v>9</v>
@@ -2674,7 +2674,7 @@
     <row r="61" spans="1:3">
       <c r="A61" s="39"/>
       <c r="B61" s="40" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C61" s="40" t="s">
         <v>14</v>
@@ -2683,7 +2683,7 @@
     <row r="62" spans="1:3">
       <c r="A62" s="39"/>
       <c r="B62" s="40" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C62" s="40" t="s">
         <v>14</v>
@@ -2692,7 +2692,7 @@
     <row r="63" spans="1:3">
       <c r="A63" s="39"/>
       <c r="B63" s="40" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C63" s="40" t="s">
         <v>9</v>
@@ -2701,7 +2701,7 @@
     <row r="64" spans="1:3">
       <c r="A64" s="39"/>
       <c r="B64" s="40" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="C64" s="40" t="s">
         <v>14</v>

</xml_diff>